<commit_message>
Boni edit daily scrum + burn down
</commit_message>
<xml_diff>
--- a/Burn down Chart.xlsx
+++ b/Burn down Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bonifasius Sinaga\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bonifasius Sinaga\Documents\TKPPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
   <si>
     <t>www.goodoldmanoj.com</t>
   </si>
@@ -234,6 +234,24 @@
   </si>
   <si>
     <t>Day 11</t>
+  </si>
+  <si>
+    <t>System Req turbo dan corel</t>
+  </si>
+  <si>
+    <t>Kelebihan dan kekurangan caldera</t>
+  </si>
+  <si>
+    <t>Edit table</t>
+  </si>
+  <si>
+    <t>Add background, edit table, link, transisi</t>
+  </si>
+  <si>
+    <t>edit number pada slide</t>
+  </si>
+  <si>
+    <t>Menyamakan seluruh tampilan tabel</t>
   </si>
 </sst>
 </file>
@@ -544,40 +562,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>21</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -627,46 +645,46 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>31</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.615384615384617</c:v>
+                  <c:v>34.153846153846153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.230769230769234</c:v>
+                  <c:v>31.307692307692307</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.84615384615385</c:v>
+                  <c:v>28.46153846153846</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.461538461538467</c:v>
+                  <c:v>25.615384615384613</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.076923076923084</c:v>
+                  <c:v>22.769230769230766</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.692307692307701</c:v>
+                  <c:v>19.92307692307692</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.307692307692315</c:v>
+                  <c:v>17.076923076923073</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.92307692307693</c:v>
+                  <c:v>14.230769230769226</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.5384615384615454</c:v>
+                  <c:v>11.38461538461538</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.1538461538461604</c:v>
+                  <c:v>8.538461538461533</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7692307692307754</c:v>
+                  <c:v>5.6923076923076863</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3846153846153908</c:v>
+                  <c:v>2.84615384615384</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2172489379008766E-15</c:v>
+                  <c:v>-6.2172489379008766E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -683,11 +701,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-199520048"/>
-        <c:axId val="-199519504"/>
+        <c:axId val="-326737536"/>
+        <c:axId val="-326736448"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-199520048"/>
+        <c:axId val="-326737536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +748,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-199519504"/>
+        <c:crossAx val="-326736448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -738,7 +756,7 @@
         <c:majorUnit val="1"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-199519504"/>
+        <c:axId val="-326736448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,7 +807,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-199520048"/>
+        <c:crossAx val="-326737536"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1713,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -1931,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -1985,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2039,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -2096,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
         <v>0</v>
@@ -2150,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -2204,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
@@ -2261,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
@@ -2315,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="4">
         <v>0</v>
@@ -2369,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
@@ -2426,7 +2444,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -2480,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="4">
         <v>0</v>
@@ -2534,7 +2552,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="4">
         <v>0</v>
@@ -2591,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="4">
         <v>0</v>
@@ -2645,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
@@ -2699,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="4">
         <v>0</v>
@@ -2753,7 +2771,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="4">
         <v>0</v>
@@ -2807,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="4">
         <v>0</v>
@@ -2864,7 +2882,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="4">
         <v>0</v>
@@ -2918,7 +2936,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="4">
         <v>0</v>
@@ -2972,7 +2990,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="4">
         <v>0</v>
@@ -3029,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="4">
         <v>0</v>
@@ -3083,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="4">
         <v>0</v>
@@ -3137,7 +3155,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="4">
         <v>0</v>
@@ -3191,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="4">
         <v>0</v>
@@ -3248,7 +3266,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" s="4">
         <v>0</v>
@@ -3302,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="M32" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32" s="4">
         <v>0</v>
@@ -3356,7 +3374,7 @@
         <v>1</v>
       </c>
       <c r="M33" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="4">
         <v>0</v>
@@ -3544,39 +3562,41 @@
       <c r="C37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="4">
         <v>0</v>
@@ -3596,39 +3616,41 @@
       <c r="C38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38" s="4">
         <v>0</v>
@@ -3648,39 +3670,41 @@
       <c r="C39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P39" s="4">
         <v>0</v>
@@ -3700,42 +3724,44 @@
       <c r="C40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="E40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q40" s="4">
         <v>0</v>
@@ -3752,42 +3778,44 @@
       <c r="C41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q41" s="4">
         <v>0</v>
@@ -3804,42 +3832,44 @@
       <c r="C42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="E42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q42" s="4">
         <v>0</v>
@@ -3857,59 +3887,59 @@
       <c r="D43" s="8"/>
       <c r="E43" s="4">
         <f>SUM(E6:E42)</f>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F43" s="5">
         <f>E43-E43/13</f>
-        <v>28.615384615384617</v>
+        <v>34.153846153846153</v>
       </c>
       <c r="G43" s="5">
         <f>F43-E43/13</f>
-        <v>26.230769230769234</v>
+        <v>31.307692307692307</v>
       </c>
       <c r="H43" s="5">
         <f>G43-E43/13</f>
-        <v>23.84615384615385</v>
+        <v>28.46153846153846</v>
       </c>
       <c r="I43" s="5">
         <f>H43-E43/13</f>
-        <v>21.461538461538467</v>
+        <v>25.615384615384613</v>
       </c>
       <c r="J43" s="5">
         <f>I43-E43/13</f>
-        <v>19.076923076923084</v>
+        <v>22.769230769230766</v>
       </c>
       <c r="K43" s="5">
         <f>J43-E43/13</f>
-        <v>16.692307692307701</v>
+        <v>19.92307692307692</v>
       </c>
       <c r="L43" s="5">
         <f>K43-E43/13</f>
-        <v>14.307692307692315</v>
+        <v>17.076923076923073</v>
       </c>
       <c r="M43" s="5">
         <f>L43-E43/13</f>
-        <v>11.92307692307693</v>
+        <v>14.230769230769226</v>
       </c>
       <c r="N43" s="5">
         <f>M43-E43/13</f>
-        <v>9.5384615384615454</v>
+        <v>11.38461538461538</v>
       </c>
       <c r="O43" s="5">
         <f>N43-E43/13</f>
-        <v>7.1538461538461604</v>
+        <v>8.538461538461533</v>
       </c>
       <c r="P43" s="5">
         <f>O43-E43/13</f>
-        <v>4.7692307692307754</v>
+        <v>5.6923076923076863</v>
       </c>
       <c r="Q43" s="5">
         <f>P43-E43/13</f>
-        <v>2.3846153846153908</v>
+        <v>2.84615384615384</v>
       </c>
       <c r="R43" s="5">
         <f>Q43-E43/13</f>
-        <v>6.2172489379008766E-15</v>
+        <v>-6.2172489379008766E-15</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -3921,51 +3951,51 @@
       <c r="D44" s="8"/>
       <c r="E44" s="4">
         <f>SUM(E6:E42)</f>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F44" s="4">
         <f>SUM(F6:F42)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" ref="G44:R44" si="0">SUM(G6:G42)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I44" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K44" s="4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L44" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M44" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N44" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O44" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P44" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q44" s="4">
         <f>SUM(Q6:Q42)</f>

</xml_diff>

<commit_message>
Boni Update Burn Down dan Daily Scrum
</commit_message>
<xml_diff>
--- a/Burn down Chart.xlsx
+++ b/Burn down Chart.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
   <si>
     <t>www.goodoldmanoj.com</t>
   </si>
@@ -249,16 +249,13 @@
   </si>
   <si>
     <t>edit number pada slide</t>
-  </si>
-  <si>
-    <t>Menyamakan seluruh tampilan tabel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +292,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -350,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -376,6 +381,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -557,48 +565,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$44:$R$44</c:f>
+              <c:f>Sheet1!$E$43:$R$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -640,51 +648,51 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$43:$R$43</c:f>
+              <c:f>Sheet1!$E$42:$R$42</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.153846153846153</c:v>
+                  <c:v>33.230769230769234</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.307692307692307</c:v>
+                  <c:v>30.461538461538463</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.46153846153846</c:v>
+                  <c:v>27.692307692307693</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.615384615384613</c:v>
+                  <c:v>24.923076923076923</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.769230769230766</c:v>
+                  <c:v>22.153846153846153</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.92307692307692</c:v>
+                  <c:v>19.384615384615383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.076923076923073</c:v>
+                  <c:v>16.615384615384613</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.230769230769226</c:v>
+                  <c:v>13.846153846153843</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.38461538461538</c:v>
+                  <c:v>11.076923076923073</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.538461538461533</c:v>
+                  <c:v>8.307692307692303</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.6923076923076863</c:v>
+                  <c:v>5.5384615384615339</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.84615384615384</c:v>
+                  <c:v>2.7692307692307647</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-6.2172489379008766E-15</c:v>
+                  <c:v>-4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -701,11 +709,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-326737536"/>
-        <c:axId val="-326736448"/>
+        <c:axId val="-2093447136"/>
+        <c:axId val="-2093461280"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-326737536"/>
+        <c:axId val="-2093447136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +756,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326736448"/>
+        <c:crossAx val="-2093461280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -756,7 +764,7 @@
         <c:majorUnit val="1"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-326736448"/>
+        <c:axId val="-2093461280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +815,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326737536"/>
+        <c:crossAx val="-2093447136"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,13 +1445,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>169206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>22411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1729,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:D43"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R77" sqref="R77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,20 +1819,48 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="E4" s="1">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1">
+        <v>31</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1">
+        <v>3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1">
+        <v>5</v>
+      </c>
+      <c r="P4" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>7</v>
+      </c>
+      <c r="R4" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1895,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -1949,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -2003,7 +2039,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2057,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -2114,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
         <v>0</v>
@@ -2168,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -2222,7 +2258,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
@@ -2279,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
@@ -2333,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="4">
         <v>0</v>
@@ -2387,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
@@ -2444,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -2498,7 +2534,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="4">
         <v>0</v>
@@ -2552,7 +2588,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="4">
         <v>0</v>
@@ -2609,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="4">
         <v>0</v>
@@ -2663,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
@@ -2717,7 +2753,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="4">
         <v>0</v>
@@ -2771,7 +2807,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="4">
         <v>0</v>
@@ -2825,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="4">
         <v>0</v>
@@ -2882,10 +2918,10 @@
         <v>1</v>
       </c>
       <c r="K24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="4">
         <v>0</v>
@@ -2936,10 +2972,10 @@
         <v>1</v>
       </c>
       <c r="K25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
@@ -2990,10 +3026,10 @@
         <v>1</v>
       </c>
       <c r="K26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="4">
         <v>0</v>
@@ -3047,10 +3083,10 @@
         <v>1</v>
       </c>
       <c r="L27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
@@ -3101,10 +3137,10 @@
         <v>1</v>
       </c>
       <c r="L28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="4">
         <v>0</v>
@@ -3155,10 +3191,10 @@
         <v>1</v>
       </c>
       <c r="L29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="4">
         <v>0</v>
@@ -3209,10 +3245,10 @@
         <v>1</v>
       </c>
       <c r="L30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="4">
         <v>0</v>
@@ -3266,10 +3302,10 @@
         <v>1</v>
       </c>
       <c r="M31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31" s="4">
         <v>0</v>
@@ -3320,10 +3356,10 @@
         <v>1</v>
       </c>
       <c r="M32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="4">
         <v>0</v>
@@ -3374,10 +3410,10 @@
         <v>1</v>
       </c>
       <c r="M33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33" s="4">
         <v>0</v>
@@ -3434,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="O34" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" s="4">
         <v>0</v>
@@ -3488,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="O35" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="4">
         <v>0</v>
@@ -3542,7 +3578,7 @@
         <v>1</v>
       </c>
       <c r="O36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36" s="4">
         <v>0</v>
@@ -3599,7 +3635,7 @@
         <v>1</v>
       </c>
       <c r="P37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="4">
         <v>0</v>
@@ -3653,7 +3689,7 @@
         <v>1</v>
       </c>
       <c r="P38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q38" s="4">
         <v>0</v>
@@ -3707,7 +3743,7 @@
         <v>1</v>
       </c>
       <c r="P39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q39" s="4">
         <v>0</v>
@@ -3764,7 +3800,7 @@
         <v>1</v>
       </c>
       <c r="Q40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="4">
         <v>0</v>
@@ -3818,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="Q41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="4">
         <v>0</v>
@@ -3826,185 +3862,151 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="B42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
       <c r="E42" s="4">
-        <v>1</v>
-      </c>
-      <c r="F42" s="4">
-        <v>1</v>
-      </c>
-      <c r="G42" s="4">
-        <v>1</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1</v>
-      </c>
-      <c r="I42" s="4">
-        <v>1</v>
-      </c>
-      <c r="J42" s="4">
-        <v>1</v>
-      </c>
-      <c r="K42" s="4">
-        <v>1</v>
-      </c>
-      <c r="L42" s="4">
-        <v>1</v>
-      </c>
-      <c r="M42" s="4">
-        <v>1</v>
-      </c>
-      <c r="N42" s="4">
-        <v>1</v>
-      </c>
-      <c r="O42" s="4">
-        <v>1</v>
-      </c>
-      <c r="P42" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="4">
-        <v>0</v>
-      </c>
-      <c r="R42" s="4">
-        <v>0</v>
+        <f>SUM(E6:E41)</f>
+        <v>36</v>
+      </c>
+      <c r="F42" s="5">
+        <f>E42-E42/13</f>
+        <v>33.230769230769234</v>
+      </c>
+      <c r="G42" s="5">
+        <f>F42-E42/13</f>
+        <v>30.461538461538463</v>
+      </c>
+      <c r="H42" s="5">
+        <f>G42-E42/13</f>
+        <v>27.692307692307693</v>
+      </c>
+      <c r="I42" s="5">
+        <f>H42-E42/13</f>
+        <v>24.923076923076923</v>
+      </c>
+      <c r="J42" s="5">
+        <f>I42-E42/13</f>
+        <v>22.153846153846153</v>
+      </c>
+      <c r="K42" s="5">
+        <f>J42-E42/13</f>
+        <v>19.384615384615383</v>
+      </c>
+      <c r="L42" s="5">
+        <f>K42-E42/13</f>
+        <v>16.615384615384613</v>
+      </c>
+      <c r="M42" s="5">
+        <f>L42-E42/13</f>
+        <v>13.846153846153843</v>
+      </c>
+      <c r="N42" s="5">
+        <f>M42-E42/13</f>
+        <v>11.076923076923073</v>
+      </c>
+      <c r="O42" s="5">
+        <f>N42-E42/13</f>
+        <v>8.307692307692303</v>
+      </c>
+      <c r="P42" s="5">
+        <f>O42-E42/13</f>
+        <v>5.5384615384615339</v>
+      </c>
+      <c r="Q42" s="5">
+        <f>P42-E42/13</f>
+        <v>2.7692307692307647</v>
+      </c>
+      <c r="R42" s="5">
+        <f>Q42-E42/13</f>
+        <v>-4.4408920985006262E-15</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="4">
-        <f>SUM(E6:E42)</f>
-        <v>37</v>
-      </c>
-      <c r="F43" s="5">
-        <f>E43-E43/13</f>
-        <v>34.153846153846153</v>
-      </c>
-      <c r="G43" s="5">
-        <f>F43-E43/13</f>
-        <v>31.307692307692307</v>
-      </c>
-      <c r="H43" s="5">
-        <f>G43-E43/13</f>
-        <v>28.46153846153846</v>
-      </c>
-      <c r="I43" s="5">
-        <f>H43-E43/13</f>
-        <v>25.615384615384613</v>
-      </c>
-      <c r="J43" s="5">
-        <f>I43-E43/13</f>
-        <v>22.769230769230766</v>
-      </c>
-      <c r="K43" s="5">
-        <f>J43-E43/13</f>
-        <v>19.92307692307692</v>
-      </c>
-      <c r="L43" s="5">
-        <f>K43-E43/13</f>
-        <v>17.076923076923073</v>
-      </c>
-      <c r="M43" s="5">
-        <f>L43-E43/13</f>
-        <v>14.230769230769226</v>
-      </c>
-      <c r="N43" s="5">
-        <f>M43-E43/13</f>
-        <v>11.38461538461538</v>
-      </c>
-      <c r="O43" s="5">
-        <f>N43-E43/13</f>
-        <v>8.538461538461533</v>
-      </c>
-      <c r="P43" s="5">
-        <f>O43-E43/13</f>
-        <v>5.6923076923076863</v>
-      </c>
-      <c r="Q43" s="5">
-        <f>P43-E43/13</f>
-        <v>2.84615384615384</v>
-      </c>
-      <c r="R43" s="5">
-        <f>Q43-E43/13</f>
-        <v>-6.2172489379008766E-15</v>
+        <f>SUM(E6:E41)</f>
+        <v>36</v>
+      </c>
+      <c r="F43" s="4">
+        <f>SUM(F6:F41)</f>
+        <v>36</v>
+      </c>
+      <c r="G43" s="4">
+        <f>SUM(G6:G41)</f>
+        <v>32</v>
+      </c>
+      <c r="H43" s="4">
+        <f>SUM(H6:H41)</f>
+        <v>29</v>
+      </c>
+      <c r="I43" s="4">
+        <f>SUM(I6:I41)</f>
+        <v>26</v>
+      </c>
+      <c r="J43" s="4">
+        <f>SUM(J6:J41)</f>
+        <v>23</v>
+      </c>
+      <c r="K43" s="4">
+        <f>SUM(K6:K41)</f>
+        <v>18</v>
+      </c>
+      <c r="L43" s="4">
+        <f>SUM(L6:L41)</f>
+        <v>18</v>
+      </c>
+      <c r="M43" s="4">
+        <f>SUM(M6:M41)</f>
+        <v>15</v>
+      </c>
+      <c r="N43" s="4">
+        <f>SUM(N6:N41)</f>
+        <v>11</v>
+      </c>
+      <c r="O43" s="4">
+        <f>SUM(O6:O41)</f>
+        <v>8</v>
+      </c>
+      <c r="P43" s="4">
+        <f>SUM(P6:P41)</f>
+        <v>5</v>
+      </c>
+      <c r="Q43" s="4">
+        <f>SUM(Q6:Q41)</f>
+        <v>2</v>
+      </c>
+      <c r="R43" s="4">
+        <f>SUM(R6:R41)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="4">
-        <f>SUM(E6:E42)</f>
-        <v>37</v>
-      </c>
-      <c r="F44" s="4">
-        <f>SUM(F6:F42)</f>
-        <v>33</v>
-      </c>
-      <c r="G44" s="4">
-        <f t="shared" ref="G44:R44" si="0">SUM(G6:G42)</f>
-        <v>30</v>
-      </c>
-      <c r="H44" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="I44" s="4">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="J44" s="4">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="K44" s="4">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L44" s="4">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="M44" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="N44" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="O44" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="P44" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="Q44" s="4">
-        <f>SUM(Q6:Q42)</f>
-        <v>0</v>
-      </c>
-      <c r="R44" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -4406,38 +4408,19 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="D3:L3"/>
+    <mergeCell ref="B42:D42"/>
     <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>